<commit_message>
(fase1:)Actualizacion duoc planilla de requerimientos
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
+++ b/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Projects\Capstone\fase1\Documentacion Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C50127-CCC3-4357-B8DD-C0B770C45313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6106A33-01BA-40F6-A353-CA0F4F4C0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2340" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimiento Inicial" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="142">
   <si>
     <t>[Nombre del Requerimiento]</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Administrador, Coordinador, Estudiante</t>
   </si>
   <si>
-    <t>El sistema debe permitir el inicio de sesión mediante usuario y contraseña encriptada.</t>
-  </si>
-  <si>
     <t>Pendiente</t>
   </si>
   <si>
@@ -238,220 +235,223 @@
     <t>Administrador</t>
   </si>
   <si>
-    <t>El sistema debe diferenciar accesos según rol (Administrador, Coordinador, Estudiante).</t>
-  </si>
-  <si>
     <t>CRUD de usuarios</t>
   </si>
   <si>
-    <t>El administrador podrá crear, modificar, eliminar y consultar usuarios registrados.</t>
-  </si>
-  <si>
     <t>CRUD de coordinadores</t>
   </si>
   <si>
-    <t>Posibilidad de administrar la información de los coordinadores académicos.</t>
-  </si>
-  <si>
     <t>CRUD de servicios</t>
   </si>
   <si>
-    <t>El sistema debe permitir administrar los servicios/actividades disponibles para reserva.</t>
-  </si>
-  <si>
     <t>CRUD de reservas</t>
   </si>
   <si>
-    <t>Permite gestionar (crear, modificar, cancelar) las reservas de horas.</t>
-  </si>
-  <si>
     <t>Consultar disponibilidad</t>
   </si>
   <si>
     <t>Estudiante, Coordinador</t>
   </si>
   <si>
-    <t>El sistema mostrará horarios disponibles para coordinar reuniones.</t>
-  </si>
-  <si>
     <t>Generación de reportes</t>
   </si>
   <si>
-    <t>El sistema debe generar reportes filtrados de reservas y usuarios en PDF/Excel.</t>
-  </si>
-  <si>
     <t>Envío de notificaciones</t>
   </si>
   <si>
-    <t>El sistema debe enviar notificaciones por correo al confirmar, modificar o cancelar una reserva.</t>
-  </si>
-  <si>
     <t>Seguridad en contraseñas</t>
   </si>
   <si>
     <t>No funcional</t>
   </si>
   <si>
-    <t>Las contraseñas deben almacenarse de forma encriptada y no visible en la base de datos.</t>
-  </si>
-  <si>
     <t>Usabilidad responsiva</t>
   </si>
   <si>
-    <t>El sistema debe adaptarse a distintos dispositivos (PC, tablet, smartphone).</t>
-  </si>
-  <si>
     <t>Disponibilidad del sistema</t>
   </si>
   <si>
-    <t>El sistema debe estar disponible 24/7 para los usuarios registrados</t>
-  </si>
-  <si>
     <t>Módulo de negocio</t>
   </si>
   <si>
     <t>Administrador, Coordinador</t>
   </si>
   <si>
-    <t>Implementación de un módulo que gestione el flujo de reservas como proceso principal.</t>
-  </si>
-  <si>
     <t>Trazabilidad de reservas</t>
   </si>
   <si>
-    <t>El sistema debe registrar historial de reservas con fechas y estados.</t>
-  </si>
-  <si>
     <t>Validación de formularios</t>
   </si>
   <si>
-    <t>Todos los formularios deben contar con validación de campos antes de guardar.</t>
-  </si>
-  <si>
     <t>Auditoría de sesiones</t>
   </si>
   <si>
-    <t>El sistema debe registrar accesos de usuarios para fines de seguridad.</t>
-  </si>
-  <si>
     <t>Recuperación de contraseña</t>
   </si>
   <si>
-    <t>Permite recuperar acceso al sistema a través de correo electrónico registrado.</t>
-  </si>
-  <si>
     <t>Perfil de usuario</t>
   </si>
   <si>
-    <t>Los usuarios podrán editar su información personal (nombre, correo, teléfono).</t>
-  </si>
-  <si>
     <t>Cambio de contraseña</t>
   </si>
   <si>
-    <t>El sistema permitirá modificar la contraseña desde la configuración de perfil.</t>
-  </si>
-  <si>
     <t>Panel de administrador</t>
   </si>
   <si>
-    <t>El administrador tendrá un panel con métricas de uso, reservas activas y usuarios.</t>
-  </si>
-  <si>
     <t>Panel de coordinador</t>
   </si>
   <si>
     <t>Coordinador</t>
   </si>
   <si>
-    <t>Los coordinadores podrán ver y gestionar sus citas en una vista de calendario.</t>
-  </si>
-  <si>
     <t>Confirmación de reserva</t>
   </si>
   <si>
     <t>Coordinador, Estudiante</t>
   </si>
   <si>
-    <t>El sistema notificará la confirmación de la reserva al estudiante y coordinador.</t>
-  </si>
-  <si>
     <t>Cancelación de reservas</t>
   </si>
   <si>
-    <t>Posibilidad de cancelar reservas con notificación automática a los implicados.</t>
-  </si>
-  <si>
     <t>Reagendamiento de reservas</t>
   </si>
   <si>
-    <t>Permite modificar la fecha/hora de una cita ya programada.</t>
-  </si>
-  <si>
     <t>Búsqueda avanzada</t>
   </si>
   <si>
-    <t>Posibilidad de buscar reservas y usuarios aplicando filtros.</t>
-  </si>
-  <si>
     <t>Exportación de historial</t>
   </si>
   <si>
-    <t>El sistema debe exportar registros de reservas e historial de usuarios a Excel/PDF.</t>
-  </si>
-  <si>
     <t>Registro de actividades</t>
   </si>
   <si>
-    <t>Guardar un log con cada acción realizada por los usuarios para auditoría.</t>
-  </si>
-  <si>
     <t>Escalabilidad</t>
   </si>
   <si>
-    <t>El sistema debe permitir aumentar usuarios concurrentes sin perder rendimiento.</t>
-  </si>
-  <si>
     <t>Tiempo de respuesta</t>
   </si>
   <si>
-    <t>El sistema debe responder a solicitudes en menos de 3 segundos.</t>
-  </si>
-  <si>
     <t>Integración con correo institucional</t>
   </si>
   <si>
-    <t>Se debe usar el correo institucional para autenticación y notificaciones.</t>
-  </si>
-  <si>
     <t>Reporte de reservas canceladas</t>
   </si>
   <si>
-    <t>El sistema debe generar reportes con las reservas canceladas y sus motivos.</t>
-  </si>
-  <si>
     <t>Reporte de disponibilidad</t>
   </si>
   <si>
-    <t>Permite generar reportes sobre la utilización de horarios.</t>
-  </si>
-  <si>
     <t>Control de concurrencia</t>
   </si>
   <si>
-    <t>Evitar que dos usuarios reserven el mismo horario simultáneamente.</t>
-  </si>
-  <si>
     <t>Interfaz amigable</t>
   </si>
   <si>
-    <t>El sistema debe tener una UI clara, sencilla y con diseño intuitivo.</t>
-  </si>
-  <si>
     <t>Compatibilidad multiplataforma</t>
   </si>
   <si>
-    <t>El sistema debe funcionar en Chrome, Edge y Firefox.</t>
+    <t>Autenticar usuarios mediante credenciales válidas (usuario y contraseña)</t>
+  </si>
+  <si>
+    <t>Gestionar roles y permisos creando, modificando o eliminando perfiles de acceso</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de usuarios almacenando datos personales, de contacto y credenciales</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de coordinadores asignando sus datos, funciones y disponibilidad</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de servicios definiendo nombre, descripción, condiciones y disponibilidad de cada servicio</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar reservas asociadas a estudiantes y coordinadores, registrando fechas, horarios y estado de confirmación</t>
+  </si>
+  <si>
+    <t>Consultar disponibilidad de horarios, servicios o recursos en tiempo real, mostrando al usuario las opciones vigentes para facilitar la planificación de reservas.</t>
+  </si>
+  <si>
+    <t>Generar reportes con filtros configurables que permitan visualizar información relevante</t>
+  </si>
+  <si>
+    <t>Enviar notificaciones automáticas por correo electrónico o mensajes a dispositivos móviles informando sobre confirmaciones, cancelaciones y recordatorios de reservas.</t>
+  </si>
+  <si>
+    <t>Garantizar seguridad en contraseñas aplicando enmascaramiento, almacenamiento encriptado y políticas de validación para proteger la información de acceso de los usuarios.</t>
+  </si>
+  <si>
+    <t>Implementar usabilidad responsiva que adapte la interfaz del sistema a distintos dispositivos (computadores, tablets y móviles), asegurando una experiencia uniforme e intuitiva.</t>
+  </si>
+  <si>
+    <t>Asegurar la disponibilidad del sistema con un nivel mínimo de servicio definido (ej. 95% de uptime), evitando interrupciones y garantizando la continuidad de las operaciones.</t>
+  </si>
+  <si>
+    <t>Implementar un módulo de negocio que gestione los procesos principales de la organización</t>
+  </si>
+  <si>
+    <t>Registrar y controlar la trazabilidad de reservas, almacenando el historial completo de creación, modificación y cancelación para garantizar transparencia y control de auditoría.</t>
+  </si>
+  <si>
+    <t>Validar formularios verificando que todos los campos obligatorios estén completos</t>
+  </si>
+  <si>
+    <t>Auditar sesiones registrando accesos, cierres de sesión y actividades realizadas por los usuarios</t>
+  </si>
+  <si>
+    <t>Recuperar contraseñas a través de un mecanismo seguro que envíe un enlace o código de verificación al correo electrónico o dispositivo móvil del usuario.</t>
+  </si>
+  <si>
+    <t>Visualizar y actualizar el perfil de usuario mostrando datos personales, información de contacto y preferencias, permitiendo su modificación controlada.</t>
+  </si>
+  <si>
+    <t>Cambiar contraseña validando la contraseña anterior y aplicando reglas de seguridad</t>
+  </si>
+  <si>
+    <t>Acceder a un panel de administrador que centralice la gestión de usuarios, coordinadores, servicios, reservas y reportes mediante una interfaz unificada.</t>
+  </si>
+  <si>
+    <t>Acceder a un panel de coordinador que permita gestionar servicios, reservas y disponibilidad, con herramientas específicas para su rol.</t>
+  </si>
+  <si>
+    <t>Confirmar reservas registradas en el sistema notificando al usuario sobre la aprobación y actualizando el estado de la misma en tiempo real.</t>
+  </si>
+  <si>
+    <t>Cancelar reservas previamente registradas actualizando su estado y notificando a los usuarios involucrados, liberando la disponibilidad de recursos.</t>
+  </si>
+  <si>
+    <t>Reagendar reservas modificando fecha y hora previamente seleccionadas, actualizando la disponibilidad y notificando a los usuarios afectados</t>
+  </si>
+  <si>
+    <t>Realizar búsquedas avanzadas aplicando filtros múltiples (usuario, fecha, servicio, estado) para localizar información de forma rápida y precisa.</t>
+  </si>
+  <si>
+    <t>Exportar historial de registros en diferentes formatos</t>
+  </si>
+  <si>
+    <t>Registrar actividades de los usuarios en un log interno que almacene acciones relevantes</t>
+  </si>
+  <si>
+    <t>Garantizar la escalabilidad del sistema permitiendo aumentar la cantidad de usuarios, servicios y transacciones sin afectar el rendimiento ni la estabilidad.</t>
+  </si>
+  <si>
+    <t>Optimizar el tiempo de respuesta de las operaciones del sistema, asegurando que las consultas y procesos se ejecuten en menos de 3 segundos en condiciones normales de carga.</t>
+  </si>
+  <si>
+    <t>Integrar el sistema con el correo institucional enviando notificaciones, confirmaciones y alertas directamente a las cuentas oficiales de los usuarios.</t>
+  </si>
+  <si>
+    <t>Generar reportes de reservas canceladas mostrando historial, motivo y fecha de cancelación, para fines de control y análisis de tendencias.</t>
+  </si>
+  <si>
+    <t>Generar reportes de disponibilidad detallando horarios, servicios y recursos libres, permitiendo la planificación anticipada por parte de los usuarios.</t>
+  </si>
+  <si>
+    <t>Controlar la concurrencia de usuarios evitando conflictos en reservas simultáneas y asegurando la consistencia de los datos en el sistema.</t>
+  </si>
+  <si>
+    <t>Diseñar una interfaz amigable con navegación intuitiva, íconos claros, mensajes de ayuda y estructura organizada para mejorar la experiencia de usuario.</t>
+  </si>
+  <si>
+    <t>Asegurar compatibilidad multiplataforma garantizando el correcto funcionamiento del sistema en distintos navegadores</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -584,8 +584,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,21 +866,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" customWidth="1"/>
-    <col min="5" max="5" width="63.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="4" max="4" width="42.54296875" customWidth="1"/>
+    <col min="5" max="5" width="115.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -902,705 +900,707 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
@@ -1655,17 +1655,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="66.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1789,7 +1789,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1797,7 +1797,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1805,7 +1805,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>

</xml_diff>

<commit_message>
docs(fase1): actualizar Mockups y Planilla de Requerimientos; eliminar carpeta NUL accidental
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
+++ b/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6106A33-01BA-40F6-A353-CA0F4F4C0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F2A97-D8A7-41F0-A8A6-94C41070B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="141">
   <si>
     <t>[Nombre del Requerimiento]</t>
   </si>
@@ -229,126 +229,27 @@
     <t>Pendiente</t>
   </si>
   <si>
-    <t>Gestión de roles y permisos</t>
-  </si>
-  <si>
     <t>Administrador</t>
   </si>
   <si>
-    <t>CRUD de usuarios</t>
-  </si>
-  <si>
-    <t>CRUD de coordinadores</t>
-  </si>
-  <si>
-    <t>CRUD de servicios</t>
-  </si>
-  <si>
-    <t>CRUD de reservas</t>
-  </si>
-  <si>
     <t>Consultar disponibilidad</t>
   </si>
   <si>
     <t>Estudiante, Coordinador</t>
   </si>
   <si>
-    <t>Generación de reportes</t>
-  </si>
-  <si>
-    <t>Envío de notificaciones</t>
-  </si>
-  <si>
-    <t>Seguridad en contraseñas</t>
-  </si>
-  <si>
     <t>No funcional</t>
   </si>
   <si>
-    <t>Usabilidad responsiva</t>
-  </si>
-  <si>
-    <t>Disponibilidad del sistema</t>
-  </si>
-  <si>
-    <t>Módulo de negocio</t>
-  </si>
-  <si>
     <t>Administrador, Coordinador</t>
   </si>
   <si>
-    <t>Trazabilidad de reservas</t>
-  </si>
-  <si>
-    <t>Validación de formularios</t>
-  </si>
-  <si>
-    <t>Auditoría de sesiones</t>
-  </si>
-  <si>
-    <t>Recuperación de contraseña</t>
-  </si>
-  <si>
-    <t>Perfil de usuario</t>
-  </si>
-  <si>
-    <t>Cambio de contraseña</t>
-  </si>
-  <si>
-    <t>Panel de administrador</t>
-  </si>
-  <si>
-    <t>Panel de coordinador</t>
-  </si>
-  <si>
     <t>Coordinador</t>
   </si>
   <si>
-    <t>Confirmación de reserva</t>
-  </si>
-  <si>
     <t>Coordinador, Estudiante</t>
   </si>
   <si>
-    <t>Cancelación de reservas</t>
-  </si>
-  <si>
-    <t>Reagendamiento de reservas</t>
-  </si>
-  <si>
-    <t>Búsqueda avanzada</t>
-  </si>
-  <si>
-    <t>Exportación de historial</t>
-  </si>
-  <si>
-    <t>Registro de actividades</t>
-  </si>
-  <si>
-    <t>Escalabilidad</t>
-  </si>
-  <si>
-    <t>Tiempo de respuesta</t>
-  </si>
-  <si>
-    <t>Integración con correo institucional</t>
-  </si>
-  <si>
-    <t>Reporte de reservas canceladas</t>
-  </si>
-  <si>
-    <t>Reporte de disponibilidad</t>
-  </si>
-  <si>
-    <t>Control de concurrencia</t>
-  </si>
-  <si>
-    <t>Interfaz amigable</t>
-  </si>
-  <si>
-    <t>Compatibilidad multiplataforma</t>
-  </si>
-  <si>
     <t>Autenticar usuarios mediante credenciales válidas (usuario y contraseña)</t>
   </si>
   <si>
@@ -452,6 +353,102 @@
   </si>
   <si>
     <t>Asegurar compatibilidad multiplataforma garantizando el correcto funcionamiento del sistema en distintos navegadores</t>
+  </si>
+  <si>
+    <t>Gestionar roles</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de usuarios</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de coordinador</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de servicios</t>
+  </si>
+  <si>
+    <t>Crear, consultar, actualizar y eliminar registros de reservas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar reportes </t>
+  </si>
+  <si>
+    <t>Enviar notificaciones</t>
+  </si>
+  <si>
+    <t>Garantizar seguridad</t>
+  </si>
+  <si>
+    <t>Implementar usabilidad responsiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asegurar la disponibilidad del sistema </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar un módulo de negocio </t>
+  </si>
+  <si>
+    <t>Registrar y controlar la trazabilidad</t>
+  </si>
+  <si>
+    <t>Validar formularios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auditar sesiones </t>
+  </si>
+  <si>
+    <t>Recuperar contraseñas</t>
+  </si>
+  <si>
+    <t>Visualizar y actualizar el perfil de usuario</t>
+  </si>
+  <si>
+    <t>Cambiar contraseña</t>
+  </si>
+  <si>
+    <t>Acceder a un panel de coordinador</t>
+  </si>
+  <si>
+    <t>Acceder a un panel administrador</t>
+  </si>
+  <si>
+    <t>Confirmar reservas</t>
+  </si>
+  <si>
+    <t>Cancelar reservas previamente registradas</t>
+  </si>
+  <si>
+    <t>Reagendar reserva</t>
+  </si>
+  <si>
+    <t>Realizar búsquedas avanzadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportar historial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrar actividades de los usuarios </t>
+  </si>
+  <si>
+    <t>Garantizar la escalabilidad del sistema</t>
+  </si>
+  <si>
+    <t>Optimizar el tiempo de respuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrar el sistema con el correo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar reportes de reservas canceladas </t>
+  </si>
+  <si>
+    <t>Generar reportes de disponibilidad detallando horarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controlar la concurrencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asegurar compatibilidad </t>
   </si>
 </sst>
 </file>
@@ -866,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,7 +911,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
@@ -925,16 +922,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
         <v>66</v>
@@ -945,16 +942,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -965,16 +962,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
         <v>66</v>
@@ -985,16 +982,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
         <v>66</v>
@@ -1005,7 +1002,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -1014,7 +1011,7 @@
         <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
         <v>66</v>
@@ -1025,16 +1022,16 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>66</v>
@@ -1045,16 +1042,16 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
         <v>66</v>
@@ -1065,16 +1062,16 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
         <v>66</v>
@@ -1085,16 +1082,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
         <v>66</v>
@@ -1105,16 +1102,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
         <v>66</v>
@@ -1125,16 +1122,16 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>66</v>
@@ -1145,16 +1142,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>66</v>
@@ -1165,16 +1162,16 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
         <v>66</v>
@@ -1185,7 +1182,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1194,7 +1191,7 @@
         <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
         <v>66</v>
@@ -1205,16 +1202,16 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>66</v>
@@ -1225,16 +1222,16 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
         <v>66</v>
@@ -1245,16 +1242,16 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="F19" t="s">
         <v>66</v>
@@ -1265,7 +1262,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1274,7 +1271,7 @@
         <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="F20" t="s">
         <v>66</v>
@@ -1285,16 +1282,16 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
         <v>66</v>
@@ -1305,16 +1302,16 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
         <v>66</v>
@@ -1325,16 +1322,16 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
         <v>66</v>
@@ -1345,16 +1342,16 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="F24" t="s">
         <v>66</v>
@@ -1365,16 +1362,16 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
         <v>66</v>
@@ -1385,16 +1382,16 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
         <v>66</v>
@@ -1405,16 +1402,16 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
         <v>66</v>
@@ -1425,16 +1422,16 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
         <v>66</v>
@@ -1445,16 +1442,16 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
         <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="F29" t="s">
         <v>66</v>
@@ -1465,16 +1462,16 @@
         <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
         <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="F30" t="s">
         <v>66</v>
@@ -1485,16 +1482,16 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
         <v>66</v>
@@ -1505,16 +1502,16 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
         <v>66</v>
@@ -1525,16 +1522,16 @@
         <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
         <v>66</v>
@@ -1545,16 +1542,16 @@
         <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
         <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
         <v>66</v>
@@ -1565,16 +1562,16 @@
         <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
         <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
         <v>66</v>
@@ -1585,16 +1582,16 @@
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
         <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="F36" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
(fase2: ajuste modulo notificaciones)
</commit_message>
<xml_diff>
--- a/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
+++ b/fase1/Documentacion Proyecto/Planilla de Requerimientos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\git\Capstone\fase1\Documentacion Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Projects\Capstone\fase1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F2A97-D8A7-41F0-A8A6-94C41070B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3D6239-C3E1-4109-A695-185ABF481F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimiento Inicial" sheetId="3" r:id="rId1"/>
@@ -455,7 +455,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -863,21 +863,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" customWidth="1"/>
-    <col min="2" max="2" width="38.08984375" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" customWidth="1"/>
-    <col min="4" max="4" width="42.54296875" customWidth="1"/>
-    <col min="5" max="5" width="115.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
+    <col min="5" max="5" width="115.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="59.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -897,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -917,7 +917,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -937,7 +937,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="24.9" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -957,7 +957,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="24.9" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -977,7 +977,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="24.9" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -997,7 +997,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="24.9" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="24.9" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="55.5" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="24.9" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="24.9" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="24.9" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="31.5" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="24.9" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="24.9" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="24.9" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>43</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
         <v>49</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
@@ -1617,7 +1617,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
@@ -1652,17 +1652,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="66.08984375" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="66.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="31.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="43.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="28.8">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="28.8">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1786,7 +1786,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1794,7 +1794,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1802,7 +1802,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="35.25" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>

</xml_diff>